<commit_message>
1. Add a table of countries and prefix of city 2.Stg repairs and Dim stage construction
</commit_message>
<xml_diff>
--- a/Tables of Project.xlsx
+++ b/Tables of Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\ETL_Process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422F9566-A78E-4AB5-9267-E297C3863D99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDF95E6-921E-4963-B033-ECF452F68434}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1DC02C89-4BFB-480E-BAE4-AA9A58C91224}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="116">
   <si>
     <t>Column Name</t>
   </si>
@@ -900,7 +900,7 @@
   <dimension ref="R2:W81"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="W83" sqref="W83"/>
+      <selection activeCell="V59" sqref="V59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>